<commit_message>
Add data import permissions
- Added so there is a permission for every type of import.
- Added so if the user doing the import dose not have access to media.browse it will not show how to upload products with images.
- Added so if the user doing the import dose not have access to create new categories it will show a list of all the avilebal categories and thellthe importer to use one/more of those categories.
- Added so if there is a supplier given to the data importer it will use that supplier insted of any other supplier.

refs JDL-14
</commit_message>
<xml_diff>
--- a/shuup_tests/importer/data/product/complex_import.xlsx
+++ b/shuup_tests/importer/data/product/complex_import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t xml:space="preserve">sku</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Manufacturer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier</t>
   </si>
   <si>
     <t xml:space="preserve">test-sku1</t>
@@ -251,12 +254,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -266,20 +269,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="5" style="0" width="23.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -313,192 +313,213 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>252</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>120.22</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>115.65</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>11500.555</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>15500.552</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J7" s="2"/>
+      <c r="K7" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>